<commit_message>
sisa bab 5 dan perhitungan(bab4)
</commit_message>
<xml_diff>
--- a/MAIN/Simulasi Excel.xlsx
+++ b/MAIN/Simulasi Excel.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester VII\Skripsi\Proposal\MAIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester VII\Skripsi\UjianMeja\MAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566E81D3-8CCC-45AF-A2DD-C11AD85CDB40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B84768-809D-472A-A783-555628A11E6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F41C27CE-65AF-4260-B115-BCA0B393B57E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F41C27CE-65AF-4260-B115-BCA0B393B57E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
   <si>
     <t>Kriteria</t>
   </si>
@@ -115,13 +116,121 @@
   </si>
   <si>
     <t>Hasil evaluasi kriteria ke – i dari alternatif x</t>
+  </si>
+  <si>
+    <t>Kehadiran</t>
+  </si>
+  <si>
+    <t>Kinerja</t>
+  </si>
+  <si>
+    <t>Kualitas Kerja</t>
+  </si>
+  <si>
+    <t>Sering Masuk</t>
+  </si>
+  <si>
+    <t>Biasa Masuk</t>
+  </si>
+  <si>
+    <t>Jarang Masuk</t>
+  </si>
+  <si>
+    <t>Tidak Pernah Masuk</t>
+  </si>
+  <si>
+    <t>Sangat Inisiatif</t>
+  </si>
+  <si>
+    <t>Cukup Inisiatif</t>
+  </si>
+  <si>
+    <t>Kurang Inisiatif</t>
+  </si>
+  <si>
+    <t>Tidak Inisiatif</t>
+  </si>
+  <si>
+    <t>Kinerja Bagus</t>
+  </si>
+  <si>
+    <t>Sangat Baik</t>
+  </si>
+  <si>
+    <t>Baik</t>
+  </si>
+  <si>
+    <t>Kurang Baik</t>
+  </si>
+  <si>
+    <t>Sangat Berkualitas</t>
+  </si>
+  <si>
+    <t>Kurang Berkualitas</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Pieter Leony MP,S.Kom</t>
+  </si>
+  <si>
+    <t>Juricho Sattya Putra,SSn</t>
+  </si>
+  <si>
+    <t>Edward Roosdartono SL,ST</t>
+  </si>
+  <si>
+    <t>Sandi Ariyadi,S,Kom</t>
+  </si>
+  <si>
+    <t>Guntur Roosminto ML Am</t>
+  </si>
+  <si>
+    <t>Irvan SM.Am</t>
+  </si>
+  <si>
+    <t>Yussi Vegillia</t>
+  </si>
+  <si>
+    <t>id_karyawan</t>
+  </si>
+  <si>
+    <t>C1(1)</t>
+  </si>
+  <si>
+    <t>C2(2)</t>
+  </si>
+  <si>
+    <t>C3(3)</t>
+  </si>
+  <si>
+    <t>C4(16)</t>
+  </si>
+  <si>
+    <t>C5(7)</t>
+  </si>
+  <si>
+    <t>Kinerja Kurang Bagus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +275,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +318,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,10 +402,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,13 +448,34 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -332,6 +484,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -347,9 +502,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{A6B51D06-EADB-48BD-A95C-6A29F30BE29A}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{9E0CB50A-01EF-4453-96BA-E199BEF414A6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -798,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3BB131A-5A3E-4E2F-8862-EFC092421637}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,11 +980,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="3">
         <v>4</v>
       </c>
@@ -837,10 +1003,10 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
@@ -859,10 +1025,10 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
@@ -881,10 +1047,10 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
@@ -903,10 +1069,10 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
@@ -925,10 +1091,10 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
@@ -944,12 +1110,12 @@
       <c r="H6" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="H8" s="7"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -960,13 +1126,13 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
       <c r="F9" s="14" t="s">
         <v>21</v>
       </c>
@@ -1050,21 +1216,21 @@
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
       <c r="N13" s="6"/>
       <c r="O13" s="7"/>
     </row>
@@ -1072,7 +1238,7 @@
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1101,7 +1267,7 @@
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="18">
         <v>3</v>
       </c>
       <c r="C15" s="4">
@@ -1130,7 +1296,7 @@
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="18">
         <v>2</v>
       </c>
       <c r="C16" s="4">
@@ -1159,7 +1325,7 @@
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="18">
         <v>1</v>
       </c>
       <c r="C17" s="4">
@@ -1202,14 +1368,14 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1328,11 +1494,11 @@
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
     </row>
     <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
@@ -1389,22 +1555,782 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A19:F19"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE1A76E-7A2D-4A42-ABE6-CD7DE60FDEB0}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.36328125" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="7" width="23.1796875" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" customWidth="1"/>
+    <col min="9" max="9" width="32.08984375" customWidth="1"/>
+    <col min="10" max="10" width="15.7265625" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="11.1796875" customWidth="1"/>
+    <col min="14" max="14" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="3">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="16"/>
+    </row>
+    <row r="8" spans="1:8" ht="42.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="B10" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="C10" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="9">
+        <f>SUM(A10:E10)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="28"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="17">
+        <v>1</v>
+      </c>
+      <c r="C14" s="16">
+        <v>2</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2</v>
+      </c>
+      <c r="E14" s="16">
+        <v>2</v>
+      </c>
+      <c r="F14" s="16">
+        <v>4</v>
+      </c>
+      <c r="G14" s="21">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="17">
+        <v>4</v>
+      </c>
+      <c r="C15" s="16">
+        <v>2</v>
+      </c>
+      <c r="D15" s="16">
+        <v>3</v>
+      </c>
+      <c r="E15" s="16">
+        <v>4</v>
+      </c>
+      <c r="F15" s="16">
+        <v>2</v>
+      </c>
+      <c r="G15" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="17">
+        <v>4</v>
+      </c>
+      <c r="C16" s="16">
+        <v>4</v>
+      </c>
+      <c r="D16" s="16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="16">
+        <v>4</v>
+      </c>
+      <c r="G16" s="17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16">
+        <v>3</v>
+      </c>
+      <c r="E17" s="16">
+        <v>2</v>
+      </c>
+      <c r="F17" s="16">
+        <v>4</v>
+      </c>
+      <c r="G17" s="17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="17">
+        <v>2</v>
+      </c>
+      <c r="C18" s="16">
+        <v>2</v>
+      </c>
+      <c r="D18" s="16">
+        <v>3</v>
+      </c>
+      <c r="E18" s="16">
+        <v>2</v>
+      </c>
+      <c r="F18" s="16">
+        <v>4</v>
+      </c>
+      <c r="G18" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="17">
+        <v>2</v>
+      </c>
+      <c r="C19" s="16">
+        <v>4</v>
+      </c>
+      <c r="D19" s="16">
+        <v>3</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4</v>
+      </c>
+      <c r="F19" s="16">
+        <v>3</v>
+      </c>
+      <c r="G19" s="17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="17">
+        <v>4</v>
+      </c>
+      <c r="C20" s="16">
+        <v>2</v>
+      </c>
+      <c r="D20" s="16">
+        <v>3</v>
+      </c>
+      <c r="E20" s="16">
+        <v>4</v>
+      </c>
+      <c r="F20" s="16">
+        <v>3</v>
+      </c>
+      <c r="G20" s="17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G24" s="36"/>
+    </row>
+    <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.4">
+      <c r="A25" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="17">
+        <f>(B14-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0</v>
+      </c>
+      <c r="C25" s="17">
+        <f t="shared" ref="C25:E25" si="0">(C14-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D25" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="17">
+        <f>(F14-MIN(F14:F20))/(MAX(F14:F20)-MIN(F14:F20))</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="17">
+        <f>(B15-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C26" s="17">
+        <f t="shared" ref="C26:F26" si="1">(C15-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D26" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E26" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="17">
+        <f>(B16-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="17">
+        <f t="shared" ref="C27:F27" si="2">(C16-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="18">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="17">
+        <f>(B17-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="17">
+        <f t="shared" ref="C28:F28" si="3">(C17-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G28" s="18">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="17">
+        <f>(B18-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C29" s="17">
+        <f t="shared" ref="C29:F29" si="4">(C18-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D29" s="17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G29" s="18">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="17">
+        <f>(B19-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C30" s="17">
+        <f t="shared" ref="C30:F30" si="5">(C19-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E30" s="17">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="17">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="G30" s="18">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="17">
+        <f>(B20-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="17">
+        <f t="shared" ref="C31:F31" si="6">(C20-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D31" s="17">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="17">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="17">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+      <c r="G31" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="36"/>
+    </row>
+    <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.4">
+      <c r="A36" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="16">
+        <f>B25*$A$10+C25*$B$10+D25*$C$10+E25*$D$10+F25*$E$10</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="23">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="16">
+        <f t="shared" ref="B37:B41" si="7">B26*$A$10+C26*$B$10+D26*$C$10+E26*$D$10+F26*$E$10</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="16">
+        <f t="shared" si="7"/>
+        <v>0.8</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="16">
+        <f t="shared" si="7"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="22">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="16">
+        <f t="shared" si="7"/>
+        <v>0.53333333333333344</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="16">
+        <f t="shared" si="7"/>
+        <v>0.76666666666666672</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="16">
+        <f>B31*$A$10+C31*$B$10+D31*$C$10+E31*$D$10+F31*$E$10</f>
+        <v>0.76666666666666672</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="22">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A12:F12"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix all done (pembimbing 1)
</commit_message>
<xml_diff>
--- a/MAIN/Simulasi Excel.xlsx
+++ b/MAIN/Simulasi Excel.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah\Semester VII\Skripsi\UjianMeja\MAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B84768-809D-472A-A783-555628A11E6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1BE0A6-FA2D-4409-B7C5-C332204331F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F41C27CE-65AF-4260-B115-BCA0B393B57E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{F41C27CE-65AF-4260-B115-BCA0B393B57E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="73">
   <si>
     <t>Kriteria</t>
   </si>
@@ -224,6 +225,27 @@
   </si>
   <si>
     <t>Kinerja Kurang Bagus</t>
+  </si>
+  <si>
+    <t>Kedisiplinan</t>
+  </si>
+  <si>
+    <t>Kepatuhan</t>
+  </si>
+  <si>
+    <t>Tanggung Jawab</t>
+  </si>
+  <si>
+    <t>Cukup</t>
+  </si>
+  <si>
+    <t>Buruk</t>
+  </si>
+  <si>
+    <t>Sangat Buruk</t>
+  </si>
+  <si>
+    <t>C4(20)</t>
   </si>
 </sst>
 </file>
@@ -328,7 +350,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -401,13 +423,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -478,6 +531,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,6 +571,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -965,7 +1054,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,11 +1069,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="3">
         <v>4</v>
       </c>
@@ -1003,10 +1092,10 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1025,10 +1114,10 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1047,10 +1136,10 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
@@ -1069,10 +1158,10 @@
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="4" t="s">
         <v>12</v>
       </c>
@@ -1091,10 +1180,10 @@
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1110,12 +1199,12 @@
       <c r="H6" s="1"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
       <c r="H8" s="7"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1126,13 +1215,13 @@
       <c r="O8" s="7"/>
     </row>
     <row r="9" spans="1:15" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
       <c r="F9" s="14" t="s">
         <v>21</v>
       </c>
@@ -1216,21 +1305,21 @@
       <c r="O12" s="7"/>
     </row>
     <row r="13" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
       <c r="N13" s="6"/>
       <c r="O13" s="7"/>
     </row>
@@ -1368,14 +1457,14 @@
       <c r="O18" s="7"/>
     </row>
     <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
+      <c r="A19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1494,11 +1583,11 @@
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
     </row>
     <row r="26" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
@@ -1519,10 +1608,7 @@
         <f>B21*$A$11+C21*$B$11+D21*$C$11+E21*$D$11+F21*$E$11</f>
         <v>0.52499999999999991</v>
       </c>
-      <c r="C27" s="2" t="str">
-        <f>IF(B27=MAX(B27:B29),"1",IF(B27=MIN(B27:B29),"3","2"))</f>
-        <v>2</v>
-      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="10" t="s">
         <v>19</v>
       </c>
@@ -1579,13 +1665,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE1A76E-7A2D-4A42-ABE6-CD7DE60FDEB0}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="35.36328125" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
     <col min="3" max="3" width="11.453125" customWidth="1"/>
     <col min="4" max="4" width="19.6328125" style="12" customWidth="1"/>
     <col min="5" max="5" width="19.90625" customWidth="1"/>
@@ -1601,11 +1688,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="3">
         <v>5</v>
       </c>
@@ -1626,10 +1713,10 @@
       <c r="A2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16" t="s">
         <v>33</v>
@@ -1648,10 +1735,10 @@
       <c r="A3" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16" t="s">
         <v>37</v>
@@ -1670,10 +1757,10 @@
       <c r="A4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16" t="s">
@@ -1688,10 +1775,10 @@
       <c r="A5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="16"/>
       <c r="E5" s="16" t="s">
         <v>42</v>
@@ -1708,10 +1795,10 @@
       <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
         <v>45</v>
@@ -1723,13 +1810,13 @@
       <c r="H6" s="16"/>
     </row>
     <row r="8" spans="1:8" ht="42.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="14" t="s">
         <v>21</v>
       </c>
@@ -1776,15 +1863,15 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="28" t="s">
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="31" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1807,7 +1894,7 @@
       <c r="F13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="28"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.4">
       <c r="A14" s="16" t="s">
@@ -1971,15 +2058,15 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36" t="s">
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2002,7 +2089,7 @@
       <c r="F24" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="36"/>
+      <c r="G24" s="39"/>
     </row>
     <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A25" s="18" t="s">
@@ -2201,12 +2288,12 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="26" t="s">
+      <c r="A34" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="36" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="39" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2220,7 +2307,7 @@
       <c r="C35" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="36"/>
+      <c r="D35" s="39"/>
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.4">
       <c r="A36" s="16" t="s">
@@ -2320,17 +2407,832 @@
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A12:F12"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A12:F12"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27887DC2-7D05-4082-B92E-A56EECEC70FB}">
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.08984375" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.26953125" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" customWidth="1"/>
+    <col min="7" max="7" width="25.26953125" customWidth="1"/>
+    <col min="8" max="8" width="24.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="3">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="11"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" ht="35.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="B10" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="26">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="9">
+        <f>SUM(A10:D10)</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+    </row>
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="39"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A14" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="27">
+        <v>5</v>
+      </c>
+      <c r="C14" s="27">
+        <v>4</v>
+      </c>
+      <c r="D14" s="27">
+        <v>3</v>
+      </c>
+      <c r="E14" s="27">
+        <v>2</v>
+      </c>
+      <c r="F14" s="23">
+        <v>29</v>
+      </c>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="27">
+        <v>1</v>
+      </c>
+      <c r="C15" s="27">
+        <v>3</v>
+      </c>
+      <c r="D15" s="27">
+        <v>4</v>
+      </c>
+      <c r="E15" s="27">
+        <v>5</v>
+      </c>
+      <c r="F15" s="27">
+        <v>30</v>
+      </c>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="27">
+        <v>1</v>
+      </c>
+      <c r="C16" s="27">
+        <v>5</v>
+      </c>
+      <c r="D16" s="27">
+        <v>2</v>
+      </c>
+      <c r="E16" s="27">
+        <v>2</v>
+      </c>
+      <c r="F16" s="27">
+        <v>35</v>
+      </c>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="27">
+        <v>1</v>
+      </c>
+      <c r="C17" s="27">
+        <v>5</v>
+      </c>
+      <c r="D17" s="27">
+        <v>5</v>
+      </c>
+      <c r="E17" s="27">
+        <v>4</v>
+      </c>
+      <c r="F17" s="27">
+        <v>36</v>
+      </c>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="27">
+        <v>4</v>
+      </c>
+      <c r="C18" s="27">
+        <v>4</v>
+      </c>
+      <c r="D18" s="27">
+        <v>5</v>
+      </c>
+      <c r="E18" s="27">
+        <v>4</v>
+      </c>
+      <c r="F18" s="27">
+        <v>37</v>
+      </c>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="27">
+        <v>5</v>
+      </c>
+      <c r="C19" s="27">
+        <v>5</v>
+      </c>
+      <c r="D19" s="27">
+        <v>1</v>
+      </c>
+      <c r="E19" s="27">
+        <v>1</v>
+      </c>
+      <c r="F19" s="27">
+        <v>38</v>
+      </c>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="27">
+        <v>5</v>
+      </c>
+      <c r="C20" s="27">
+        <v>4</v>
+      </c>
+      <c r="D20" s="27">
+        <v>5</v>
+      </c>
+      <c r="E20" s="27">
+        <v>1</v>
+      </c>
+      <c r="F20" s="27">
+        <v>50</v>
+      </c>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="39"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A25" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="27">
+        <f>(B14-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="27">
+        <f t="shared" ref="C25:E25" si="0">(C14-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="27">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="27">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="F25" s="23">
+        <v>29</v>
+      </c>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="27">
+        <f>(B15-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0</v>
+      </c>
+      <c r="C26" s="27">
+        <f t="shared" ref="C26:E26" si="1">(C15-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="E26" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="27">
+        <v>30</v>
+      </c>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="27">
+        <f>(B16-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0</v>
+      </c>
+      <c r="C27" s="27">
+        <f t="shared" ref="C27:E27" si="2">(C16-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="27">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="E27" s="27">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="F27" s="27">
+        <v>35</v>
+      </c>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="27">
+        <f>(B17-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="27">
+        <f t="shared" ref="C28:E28" si="3">(C17-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>1</v>
+      </c>
+      <c r="D28" s="27">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="27">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="F28" s="27">
+        <v>36</v>
+      </c>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="27">
+        <f>(B18-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>0.75</v>
+      </c>
+      <c r="C29" s="27">
+        <f t="shared" ref="C29:E29" si="4">(C18-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="27">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="27">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="F29" s="27">
+        <v>37</v>
+      </c>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="27">
+        <f>(B19-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="27">
+        <f t="shared" ref="C30:E30" si="5">(C19-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>1</v>
+      </c>
+      <c r="D30" s="27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="27">
+        <v>38</v>
+      </c>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="27">
+        <f>(B20-MIN(B14:B20))/(MAX(B14:B20)-MIN(B14:B20))</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="27">
+        <f t="shared" ref="C31:E31" si="6">(C20-MIN(C14:C20))/(MAX(C14:C20)-MIN(C14:C20))</f>
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="27">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="27">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="27">
+        <v>50</v>
+      </c>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+    </row>
+    <row r="34" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="39"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+    </row>
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.4">
+      <c r="A36" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="26">
+        <f t="shared" ref="B36:B42" si="7">B25*$A$10+C25*$B$10+D25*$C$10+E25*$D$10</f>
+        <v>0.5625</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="23">
+        <v>29</v>
+      </c>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+    </row>
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="26">
+        <f t="shared" si="7"/>
+        <v>0.4375</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27">
+        <v>30</v>
+      </c>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+    </row>
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="26">
+        <f t="shared" si="7"/>
+        <v>0.375</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27">
+        <v>35</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+    </row>
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="26">
+        <f t="shared" si="7"/>
+        <v>0.6875</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27">
+        <v>36</v>
+      </c>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+    </row>
+    <row r="40" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="26">
+        <f t="shared" si="7"/>
+        <v>0.75</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27">
+        <v>37</v>
+      </c>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+    </row>
+    <row r="41" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="26">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27">
+        <v>38</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+    </row>
+    <row r="42" spans="1:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="26">
+        <f t="shared" si="7"/>
+        <v>0.625</v>
+      </c>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27">
+        <v>50</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A23:E23"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>